<commit_message>
fixing results to account for x2 error
</commit_message>
<xml_diff>
--- a/csc445hw01Results.xlsx
+++ b/csc445hw01Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cedrichansen/Programs/csc445hw01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D699C2DF-2B90-9C48-8DA6-251907C71F04}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1356D57D-87DE-EC4E-BC17-24C8B70F559B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{81977BFE-FBD4-7846-A2CF-47553195A17A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14900" xr2:uid="{81977BFE-FBD4-7846-A2CF-47553195A17A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="28">
   <si>
     <t>Trial</t>
   </si>
@@ -111,13 +111,10 @@
     <t>UDP Interaction</t>
   </si>
   <si>
-    <t>trial 3</t>
-  </si>
-  <si>
     <t>Note: everything was run 5 times and averaged</t>
   </si>
   <si>
-    <t>Andy Vadnais Laptop (off campus)</t>
+    <t>John Santos' Laptop (off campus)</t>
   </si>
 </sst>
 </file>
@@ -185,55 +182,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CFF44F2-52DD-2A4E-8BB5-7FE511E6C990}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="825500" y="8331200"/>
-          <a:ext cx="8267700" cy="5384800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -533,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451A1E80-CBA9-F747-A72D-EF20C4DCD04D}">
-  <dimension ref="A4:H40"/>
+  <dimension ref="A4:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,7 +533,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -633,7 +581,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -709,10 +657,10 @@
         <v>16</v>
       </c>
       <c r="F19">
-        <v>4.5933237</v>
+        <v>9.1866474</v>
       </c>
       <c r="H19">
-        <v>2.1095704999999998</v>
+        <v>4.2191409999999996</v>
       </c>
     </row>
     <row r="20" spans="5:8" x14ac:dyDescent="0.2">
@@ -720,10 +668,10 @@
         <v>17</v>
       </c>
       <c r="F20">
-        <v>5.7056417000000001</v>
+        <v>11.4112834</v>
       </c>
       <c r="H20">
-        <v>4.7080200000000003</v>
+        <v>9.4160400000000006</v>
       </c>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.2">
@@ -731,10 +679,10 @@
         <v>18</v>
       </c>
       <c r="F21">
-        <v>7.1572046</v>
+        <v>14.3144092</v>
       </c>
       <c r="H21">
-        <v>6.1960397</v>
+        <v>12.3920794</v>
       </c>
     </row>
     <row r="22" spans="5:8" x14ac:dyDescent="0.2">
@@ -742,10 +690,10 @@
         <v>19</v>
       </c>
       <c r="F22">
-        <v>8.6912780000000005</v>
+        <v>17.382556000000001</v>
       </c>
       <c r="H22">
-        <v>6.7530913000000004</v>
+        <v>13.506182600000001</v>
       </c>
     </row>
     <row r="23" spans="5:8" x14ac:dyDescent="0.2">
@@ -753,10 +701,10 @@
         <v>20</v>
       </c>
       <c r="F23">
-        <v>9.5899920000000005</v>
+        <v>19.179984000000001</v>
       </c>
       <c r="H23">
-        <v>6.8946047000000004</v>
+        <v>13.789209400000001</v>
       </c>
     </row>
     <row r="25" spans="5:8" x14ac:dyDescent="0.2">
@@ -824,7 +772,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E33" s="3" t="s">
         <v>22</v>
       </c>
@@ -835,7 +783,7 @@
         <v>2381</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E34" t="s">
         <v>23</v>
       </c>
@@ -846,7 +794,7 @@
         <v>4718</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E35" t="s">
         <v>24</v>
       </c>
@@ -857,13 +805,7 @@
         <v>9684</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>26</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>